<commit_message>
docs: add image of dynamic to report
</commit_message>
<xml_diff>
--- a/speedup-analyse-dynamic.xlsx
+++ b/speedup-analyse-dynamic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\user\CLionProjects\fh-ppr-mandelbrot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94D686C6-15FB-4EA3-908A-D01AC58B16EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA814A38-EBF0-4D3D-8646-9B8DB0C84FDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5880" yWindow="1590" windowWidth="28800" windowHeight="11505" activeTab="1" xr2:uid="{63552AAE-C5A2-4ED5-98F5-496E86A19847}"/>
+    <workbookView xWindow="1410" yWindow="1860" windowWidth="26400" windowHeight="12120" xr2:uid="{63552AAE-C5A2-4ED5-98F5-496E86A19847}"/>
   </bookViews>
   <sheets>
     <sheet name="maxIterations = 100" sheetId="2" r:id="rId1"/>
@@ -985,10 +985,10 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>'maxIterations = 100'!$B$104:$I$104</c:f>
+              <c:f>'maxIterations = 100'!$B$104:$Q$104</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1012,6 +1012,30 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>3.3068870315000338</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.3738065998308189</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.5557701158319626</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.3454153920009722</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.4481396905983379</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.5015561730858487</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.5602772478251326</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.4527856181824594</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.1484856401778845</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1841,8 +1865,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="3.0303030303030304E-2"/>
-              <c:y val="0.32578556712668982"/>
+              <c:x val="1.9741967897577158E-2"/>
+              <c:y val="0.29188724290819579"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -7696,20 +7720,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EE43085-64B6-48E6-B0EF-CBACF6AF9272}">
   <dimension ref="A1:Q104"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U147" sqref="U147"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M126" sqref="M126"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="8" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="17" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="8" width="18.265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.73046875" bestFit="1" customWidth="1"/>
+    <col min="10" max="17" width="18.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>0</v>
@@ -7760,7 +7784,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
         <v>20</v>
       </c>
@@ -7813,7 +7837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B3">
         <v>0.58803700000000003</v>
       </c>
@@ -7863,7 +7887,7 @@
         <v>0.132852</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B4">
         <v>0.42796800000000002</v>
       </c>
@@ -7913,7 +7937,7 @@
         <v>0.13026699999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B5">
         <v>0.43537599999999999</v>
       </c>
@@ -7963,7 +7987,7 @@
         <v>0.12875300000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B6">
         <v>0.42943599999999998</v>
       </c>
@@ -8013,7 +8037,7 @@
         <v>0.12891</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B7">
         <v>0.43421599999999999</v>
       </c>
@@ -8063,7 +8087,7 @@
         <v>0.130389</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B8">
         <v>0.43825900000000001</v>
       </c>
@@ -8113,7 +8137,7 @@
         <v>0.13509499999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B9">
         <v>0.438496</v>
       </c>
@@ -8163,7 +8187,7 @@
         <v>0.12934100000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B10">
         <v>0.426977</v>
       </c>
@@ -8213,7 +8237,7 @@
         <v>0.12803400000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B11">
         <v>0.42899199999999998</v>
       </c>
@@ -8263,7 +8287,7 @@
         <v>0.12775800000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B12">
         <v>0.43338500000000002</v>
       </c>
@@ -8313,7 +8337,7 @@
         <v>0.12764</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B13">
         <v>0.43303999999999998</v>
       </c>
@@ -8363,7 +8387,7 @@
         <v>0.13564300000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B14">
         <v>0.43541000000000002</v>
       </c>
@@ -8413,7 +8437,7 @@
         <v>0.141962</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B15">
         <v>0.42666199999999999</v>
       </c>
@@ -8463,7 +8487,7 @@
         <v>0.14182600000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B16">
         <v>0.43084899999999998</v>
       </c>
@@ -8513,7 +8537,7 @@
         <v>0.14207500000000001</v>
       </c>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B17">
         <v>0.425174</v>
       </c>
@@ -8563,7 +8587,7 @@
         <v>0.141425</v>
       </c>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B18">
         <v>0.42555500000000002</v>
       </c>
@@ -8613,7 +8637,7 @@
         <v>0.14380699999999999</v>
       </c>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B19">
         <v>0.43152099999999999</v>
       </c>
@@ -8663,7 +8687,7 @@
         <v>0.14163400000000001</v>
       </c>
     </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B20">
         <v>0.431282</v>
       </c>
@@ -8713,7 +8737,7 @@
         <v>0.139714</v>
       </c>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B21">
         <v>0.42931799999999998</v>
       </c>
@@ -8763,7 +8787,7 @@
         <v>0.14010400000000001</v>
       </c>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B22">
         <v>0.426172</v>
       </c>
@@ -8813,7 +8837,7 @@
         <v>0.14161299999999999</v>
       </c>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B23">
         <v>0.42931200000000003</v>
       </c>
@@ -8863,7 +8887,7 @@
         <v>0.14020299999999999</v>
       </c>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B24">
         <v>0.42585400000000001</v>
       </c>
@@ -8913,7 +8937,7 @@
         <v>0.14096</v>
       </c>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B25">
         <v>0.42701800000000001</v>
       </c>
@@ -8963,7 +8987,7 @@
         <v>0.139877</v>
       </c>
     </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B26">
         <v>0.43287799999999999</v>
       </c>
@@ -9013,7 +9037,7 @@
         <v>0.14019100000000001</v>
       </c>
     </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B27">
         <v>0.42793700000000001</v>
       </c>
@@ -9063,7 +9087,7 @@
         <v>0.14297899999999999</v>
       </c>
     </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B28">
         <v>0.43178100000000003</v>
       </c>
@@ -9113,7 +9137,7 @@
         <v>0.14007800000000001</v>
       </c>
     </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B29">
         <v>0.42638100000000001</v>
       </c>
@@ -9163,7 +9187,7 @@
         <v>0.141987</v>
       </c>
     </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B30">
         <v>0.43647599999999998</v>
       </c>
@@ -9213,7 +9237,7 @@
         <v>0.140043</v>
       </c>
     </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B31">
         <v>0.42365599999999998</v>
       </c>
@@ -9263,7 +9287,7 @@
         <v>0.13868</v>
       </c>
     </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B32">
         <v>0.43129200000000001</v>
       </c>
@@ -9313,7 +9337,7 @@
         <v>0.13908899999999999</v>
       </c>
     </row>
-    <row r="33" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B33">
         <v>0.43032100000000001</v>
       </c>
@@ -9363,7 +9387,7 @@
         <v>0.14114299999999999</v>
       </c>
     </row>
-    <row r="34" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B34">
         <v>0.42694300000000002</v>
       </c>
@@ -9413,7 +9437,7 @@
         <v>0.139929</v>
       </c>
     </row>
-    <row r="35" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B35">
         <v>0.43042200000000003</v>
       </c>
@@ -9463,7 +9487,7 @@
         <v>0.14085600000000001</v>
       </c>
     </row>
-    <row r="36" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B36">
         <v>0.42617500000000003</v>
       </c>
@@ -9513,7 +9537,7 @@
         <v>0.14249300000000001</v>
       </c>
     </row>
-    <row r="37" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B37">
         <v>0.42782999999999999</v>
       </c>
@@ -9563,7 +9587,7 @@
         <v>0.14094899999999999</v>
       </c>
     </row>
-    <row r="38" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B38">
         <v>0.42320200000000002</v>
       </c>
@@ -9613,7 +9637,7 @@
         <v>0.15079699999999999</v>
       </c>
     </row>
-    <row r="39" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B39">
         <v>0.423508</v>
       </c>
@@ -9663,7 +9687,7 @@
         <v>0.13972499999999999</v>
       </c>
     </row>
-    <row r="40" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B40">
         <v>0.446324</v>
       </c>
@@ -9713,7 +9737,7 @@
         <v>0.14074</v>
       </c>
     </row>
-    <row r="41" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B41">
         <v>0.42313600000000001</v>
       </c>
@@ -9763,7 +9787,7 @@
         <v>0.13935700000000001</v>
       </c>
     </row>
-    <row r="42" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B42">
         <v>0.432556</v>
       </c>
@@ -9813,7 +9837,7 @@
         <v>0.141099</v>
       </c>
     </row>
-    <row r="43" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B43">
         <v>0.42398000000000002</v>
       </c>
@@ -9863,7 +9887,7 @@
         <v>0.145065</v>
       </c>
     </row>
-    <row r="44" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B44">
         <v>0.42751299999999998</v>
       </c>
@@ -9913,7 +9937,7 @@
         <v>0.14039299999999999</v>
       </c>
     </row>
-    <row r="45" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B45">
         <v>0.42898500000000001</v>
       </c>
@@ -9963,7 +9987,7 @@
         <v>0.14054900000000001</v>
       </c>
     </row>
-    <row r="46" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B46">
         <v>0.42500399999999999</v>
       </c>
@@ -10013,7 +10037,7 @@
         <v>0.141039</v>
       </c>
     </row>
-    <row r="47" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B47">
         <v>0.43889600000000001</v>
       </c>
@@ -10063,7 +10087,7 @@
         <v>0.140155</v>
       </c>
     </row>
-    <row r="48" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B48">
         <v>0.42940699999999998</v>
       </c>
@@ -10113,7 +10137,7 @@
         <v>0.13958699999999999</v>
       </c>
     </row>
-    <row r="49" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B49">
         <v>0.43026500000000001</v>
       </c>
@@ -10163,7 +10187,7 @@
         <v>0.141788</v>
       </c>
     </row>
-    <row r="50" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B50">
         <v>0.42362100000000003</v>
       </c>
@@ -10213,7 +10237,7 @@
         <v>0.143288</v>
       </c>
     </row>
-    <row r="51" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B51">
         <v>0.43774299999999999</v>
       </c>
@@ -10263,7 +10287,7 @@
         <v>0.14020299999999999</v>
       </c>
     </row>
-    <row r="52" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B52">
         <v>0.42732799999999999</v>
       </c>
@@ -10313,7 +10337,7 @@
         <v>0.141121</v>
       </c>
     </row>
-    <row r="53" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B53">
         <v>0.42397400000000002</v>
       </c>
@@ -10363,7 +10387,7 @@
         <v>0.13949700000000001</v>
       </c>
     </row>
-    <row r="54" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B54">
         <v>0.42979899999999999</v>
       </c>
@@ -10413,7 +10437,7 @@
         <v>0.127192</v>
       </c>
     </row>
-    <row r="55" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B55">
         <v>0.42280600000000002</v>
       </c>
@@ -10463,7 +10487,7 @@
         <v>0.12743499999999999</v>
       </c>
     </row>
-    <row r="56" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B56">
         <v>0.42938100000000001</v>
       </c>
@@ -10513,7 +10537,7 @@
         <v>0.126751</v>
       </c>
     </row>
-    <row r="57" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B57">
         <v>0.43348199999999998</v>
       </c>
@@ -10563,7 +10587,7 @@
         <v>0.128076</v>
       </c>
     </row>
-    <row r="58" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B58">
         <v>0.43395499999999998</v>
       </c>
@@ -10613,7 +10637,7 @@
         <v>0.128113</v>
       </c>
     </row>
-    <row r="59" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B59">
         <v>0.42664800000000003</v>
       </c>
@@ -10663,7 +10687,7 @@
         <v>0.12928100000000001</v>
       </c>
     </row>
-    <row r="60" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B60">
         <v>0.426649</v>
       </c>
@@ -10713,7 +10737,7 @@
         <v>0.12709599999999999</v>
       </c>
     </row>
-    <row r="61" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B61">
         <v>0.42689899999999997</v>
       </c>
@@ -10763,7 +10787,7 @@
         <v>0.130109</v>
       </c>
     </row>
-    <row r="62" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B62">
         <v>0.42236099999999999</v>
       </c>
@@ -10813,7 +10837,7 @@
         <v>0.12618799999999999</v>
       </c>
     </row>
-    <row r="63" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B63">
         <v>0.42630699999999999</v>
       </c>
@@ -10863,7 +10887,7 @@
         <v>0.126411</v>
       </c>
     </row>
-    <row r="64" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B64">
         <v>0.42912800000000001</v>
       </c>
@@ -10913,7 +10937,7 @@
         <v>0.12687399999999999</v>
       </c>
     </row>
-    <row r="65" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B65">
         <v>0.43276599999999998</v>
       </c>
@@ -10963,7 +10987,7 @@
         <v>0.12957099999999999</v>
       </c>
     </row>
-    <row r="66" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B66">
         <v>0.42416300000000001</v>
       </c>
@@ -11013,7 +11037,7 @@
         <v>0.12587400000000001</v>
       </c>
     </row>
-    <row r="67" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B67">
         <v>0.42562</v>
       </c>
@@ -11063,7 +11087,7 @@
         <v>0.126304</v>
       </c>
     </row>
-    <row r="68" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B68">
         <v>0.425985</v>
       </c>
@@ -11113,7 +11137,7 @@
         <v>0.12753999999999999</v>
       </c>
     </row>
-    <row r="69" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B69">
         <v>0.42482500000000001</v>
       </c>
@@ -11163,7 +11187,7 @@
         <v>0.12646099999999999</v>
       </c>
     </row>
-    <row r="70" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B70">
         <v>0.42860399999999998</v>
       </c>
@@ -11213,7 +11237,7 @@
         <v>0.12679000000000001</v>
       </c>
     </row>
-    <row r="71" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B71">
         <v>0.42527300000000001</v>
       </c>
@@ -11263,7 +11287,7 @@
         <v>0.12642400000000001</v>
       </c>
     </row>
-    <row r="72" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B72">
         <v>0.42739899999999997</v>
       </c>
@@ -11313,7 +11337,7 @@
         <v>0.12948999999999999</v>
       </c>
     </row>
-    <row r="73" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B73">
         <v>0.424564</v>
       </c>
@@ -11363,7 +11387,7 @@
         <v>0.13112599999999999</v>
       </c>
     </row>
-    <row r="74" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B74">
         <v>0.42701600000000001</v>
       </c>
@@ -11413,7 +11437,7 @@
         <v>0.127361</v>
       </c>
     </row>
-    <row r="75" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B75">
         <v>0.42896000000000001</v>
       </c>
@@ -11463,7 +11487,7 @@
         <v>0.126863</v>
       </c>
     </row>
-    <row r="76" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B76">
         <v>0.43364999999999998</v>
       </c>
@@ -11513,7 +11537,7 @@
         <v>0.12657099999999999</v>
       </c>
     </row>
-    <row r="77" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B77">
         <v>0.42809999999999998</v>
       </c>
@@ -11563,7 +11587,7 @@
         <v>0.12764400000000001</v>
       </c>
     </row>
-    <row r="78" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B78">
         <v>0.42585000000000001</v>
       </c>
@@ -11613,7 +11637,7 @@
         <v>0.126305</v>
       </c>
     </row>
-    <row r="79" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B79">
         <v>0.42642400000000003</v>
       </c>
@@ -11663,7 +11687,7 @@
         <v>0.13167999999999999</v>
       </c>
     </row>
-    <row r="80" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B80">
         <v>0.42482799999999998</v>
       </c>
@@ -11713,7 +11737,7 @@
         <v>0.140847</v>
       </c>
     </row>
-    <row r="81" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B81">
         <v>0.42541400000000001</v>
       </c>
@@ -11763,7 +11787,7 @@
         <v>0.13961499999999999</v>
       </c>
     </row>
-    <row r="82" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B82">
         <v>0.42849399999999999</v>
       </c>
@@ -11813,7 +11837,7 @@
         <v>0.13907</v>
       </c>
     </row>
-    <row r="83" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B83">
         <v>0.42532700000000001</v>
       </c>
@@ -11863,7 +11887,7 @@
         <v>0.13928599999999999</v>
       </c>
     </row>
-    <row r="84" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B84">
         <v>0.431035</v>
       </c>
@@ -11913,7 +11937,7 @@
         <v>0.13869200000000001</v>
       </c>
     </row>
-    <row r="85" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B85">
         <v>0.42305700000000002</v>
       </c>
@@ -11963,7 +11987,7 @@
         <v>0.13938500000000001</v>
       </c>
     </row>
-    <row r="86" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B86">
         <v>0.42962400000000001</v>
       </c>
@@ -12013,7 +12037,7 @@
         <v>0.14139599999999999</v>
       </c>
     </row>
-    <row r="87" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B87">
         <v>0.423037</v>
       </c>
@@ -12063,7 +12087,7 @@
         <v>0.139351</v>
       </c>
     </row>
-    <row r="88" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B88">
         <v>0.42401800000000001</v>
       </c>
@@ -12113,7 +12137,7 @@
         <v>0.143096</v>
       </c>
     </row>
-    <row r="89" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B89">
         <v>0.43085699999999999</v>
       </c>
@@ -12163,7 +12187,7 @@
         <v>0.14061100000000001</v>
       </c>
     </row>
-    <row r="90" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B90">
         <v>0.429288</v>
       </c>
@@ -12213,7 +12237,7 @@
         <v>0.140872</v>
       </c>
     </row>
-    <row r="91" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B91">
         <v>0.43176900000000001</v>
       </c>
@@ -12263,7 +12287,7 @@
         <v>0.14266000000000001</v>
       </c>
     </row>
-    <row r="92" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B92">
         <v>0.42543999999999998</v>
       </c>
@@ -12313,7 +12337,7 @@
         <v>0.14104800000000001</v>
       </c>
     </row>
-    <row r="93" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B93">
         <v>0.432861</v>
       </c>
@@ -12363,7 +12387,7 @@
         <v>0.14149999999999999</v>
       </c>
     </row>
-    <row r="94" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B94">
         <v>0.422954</v>
       </c>
@@ -12413,7 +12437,7 @@
         <v>0.13941100000000001</v>
       </c>
     </row>
-    <row r="95" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B95">
         <v>0.42286899999999999</v>
       </c>
@@ -12463,7 +12487,7 @@
         <v>0.14211399999999999</v>
       </c>
     </row>
-    <row r="96" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B96">
         <v>0.42887599999999998</v>
       </c>
@@ -12513,7 +12537,7 @@
         <v>0.13891899999999999</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B97">
         <v>0.42381400000000002</v>
       </c>
@@ -12563,7 +12587,7 @@
         <v>0.139429</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B98">
         <v>0.42910199999999998</v>
       </c>
@@ -12613,7 +12637,7 @@
         <v>0.13911699999999999</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B99">
         <v>0.42360199999999998</v>
       </c>
@@ -12663,7 +12687,7 @@
         <v>0.139377</v>
       </c>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B100">
         <v>0.42852499999999999</v>
       </c>
@@ -12713,7 +12737,7 @@
         <v>0.15018500000000001</v>
       </c>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B101">
         <v>0.42718899999999999</v>
       </c>
@@ -12763,7 +12787,7 @@
         <v>0.15251799999999999</v>
       </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B102">
         <v>0.42636099999999999</v>
       </c>
@@ -12813,7 +12837,7 @@
         <v>0.150058</v>
       </c>
     </row>
-    <row r="103" spans="1:17" ht="21" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:17" ht="21" x14ac:dyDescent="0.65">
       <c r="A103" s="1" t="s">
         <v>9</v>
       </c>
@@ -12882,7 +12906,7 @@
         <v>0.13660789000000001</v>
       </c>
     </row>
-    <row r="104" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:17" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" s="1" t="s">
         <v>10</v>
       </c>
@@ -12963,18 +12987,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABC6FA6B-6BAC-4EAE-AB2E-F345630EEEFF}">
   <dimension ref="A1:Q104"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3:Q102"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A119" sqref="A119"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="17" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="17" width="19.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>0</v>
@@ -13025,7 +13049,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
         <v>20</v>
       </c>
@@ -13078,7 +13102,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B3">
         <v>1.5942099999999999</v>
       </c>
@@ -13128,7 +13152,7 @@
         <v>0.27827600000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B4">
         <v>1.58511</v>
       </c>
@@ -13178,7 +13202,7 @@
         <v>0.27484900000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B5">
         <v>1.58504</v>
       </c>
@@ -13228,7 +13252,7 @@
         <v>0.27440300000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B6">
         <v>1.5851500000000001</v>
       </c>
@@ -13278,7 +13302,7 @@
         <v>0.27506799999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B7">
         <v>1.58633</v>
       </c>
@@ -13328,7 +13352,7 @@
         <v>0.27659899999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B8">
         <v>1.58087</v>
       </c>
@@ -13378,7 +13402,7 @@
         <v>0.27618999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B9">
         <v>1.59046</v>
       </c>
@@ -13428,7 +13452,7 @@
         <v>0.280829</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B10">
         <v>1.5825400000000001</v>
       </c>
@@ -13478,7 +13502,7 @@
         <v>0.279802</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B11">
         <v>1.5881099999999999</v>
       </c>
@@ -13528,7 +13552,7 @@
         <v>0.284076</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B12">
         <v>1.5999399999999999</v>
       </c>
@@ -13578,7 +13602,7 @@
         <v>0.28621799999999997</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B13">
         <v>1.5846199999999999</v>
       </c>
@@ -13628,7 +13652,7 @@
         <v>0.288574</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B14">
         <v>1.5862499999999999</v>
       </c>
@@ -13678,7 +13702,7 @@
         <v>0.281163</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B15">
         <v>1.5883499999999999</v>
       </c>
@@ -13728,7 +13752,7 @@
         <v>0.27167999999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B16">
         <v>1.5846100000000001</v>
       </c>
@@ -13778,7 +13802,7 @@
         <v>0.27696799999999999</v>
       </c>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B17">
         <v>1.5855600000000001</v>
       </c>
@@ -13828,7 +13852,7 @@
         <v>0.27504200000000001</v>
       </c>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B18">
         <v>1.5747500000000001</v>
       </c>
@@ -13878,7 +13902,7 @@
         <v>0.27345900000000001</v>
       </c>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B19">
         <v>1.5806199999999999</v>
       </c>
@@ -13928,7 +13952,7 @@
         <v>0.28617199999999998</v>
       </c>
     </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B20">
         <v>1.5756300000000001</v>
       </c>
@@ -13978,7 +14002,7 @@
         <v>0.29871999999999999</v>
       </c>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B21">
         <v>1.5747100000000001</v>
       </c>
@@ -14028,7 +14052,7 @@
         <v>0.27450400000000003</v>
       </c>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B22">
         <v>1.5779099999999999</v>
       </c>
@@ -14078,7 +14102,7 @@
         <v>0.27332899999999999</v>
       </c>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B23">
         <v>1.5788800000000001</v>
       </c>
@@ -14128,7 +14152,7 @@
         <v>0.27868199999999999</v>
       </c>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B24">
         <v>1.5731200000000001</v>
       </c>
@@ -14178,7 +14202,7 @@
         <v>0.27581699999999998</v>
       </c>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B25">
         <v>1.5768200000000001</v>
       </c>
@@ -14228,7 +14252,7 @@
         <v>0.27162999999999998</v>
       </c>
     </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B26">
         <v>1.57595</v>
       </c>
@@ -14278,7 +14302,7 @@
         <v>0.27285900000000002</v>
       </c>
     </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B27">
         <v>1.58114</v>
       </c>
@@ -14328,7 +14352,7 @@
         <v>0.279532</v>
       </c>
     </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B28">
         <v>1.57531</v>
       </c>
@@ -14378,7 +14402,7 @@
         <v>0.27374900000000002</v>
       </c>
     </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B29">
         <v>1.57629</v>
       </c>
@@ -14428,7 +14452,7 @@
         <v>0.270345</v>
       </c>
     </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B30">
         <v>1.5810500000000001</v>
       </c>
@@ -14478,7 +14502,7 @@
         <v>0.278111</v>
       </c>
     </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B31">
         <v>1.5808599999999999</v>
       </c>
@@ -14528,7 +14552,7 @@
         <v>0.282524</v>
       </c>
     </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B32">
         <v>1.5775699999999999</v>
       </c>
@@ -14578,7 +14602,7 @@
         <v>0.27395199999999997</v>
       </c>
     </row>
-    <row r="33" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B33">
         <v>1.5986199999999999</v>
       </c>
@@ -14628,7 +14652,7 @@
         <v>0.27410899999999999</v>
       </c>
     </row>
-    <row r="34" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B34">
         <v>1.57396</v>
       </c>
@@ -14678,7 +14702,7 @@
         <v>0.28113900000000003</v>
       </c>
     </row>
-    <row r="35" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B35">
         <v>1.5742700000000001</v>
       </c>
@@ -14728,7 +14752,7 @@
         <v>0.277729</v>
       </c>
     </row>
-    <row r="36" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B36">
         <v>1.59243</v>
       </c>
@@ -14778,7 +14802,7 @@
         <v>0.27473700000000001</v>
       </c>
     </row>
-    <row r="37" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B37">
         <v>1.5902099999999999</v>
       </c>
@@ -14828,7 +14852,7 @@
         <v>0.27753</v>
       </c>
     </row>
-    <row r="38" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B38">
         <v>1.5942400000000001</v>
       </c>
@@ -14878,7 +14902,7 @@
         <v>0.28082699999999999</v>
       </c>
     </row>
-    <row r="39" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B39">
         <v>1.5850200000000001</v>
       </c>
@@ -14928,7 +14952,7 @@
         <v>0.277221</v>
       </c>
     </row>
-    <row r="40" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B40">
         <v>1.57887</v>
       </c>
@@ -14978,7 +15002,7 @@
         <v>0.275447</v>
       </c>
     </row>
-    <row r="41" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B41">
         <v>1.57592</v>
       </c>
@@ -15028,7 +15052,7 @@
         <v>0.280752</v>
       </c>
     </row>
-    <row r="42" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B42">
         <v>1.57745</v>
       </c>
@@ -15078,7 +15102,7 @@
         <v>0.27944999999999998</v>
       </c>
     </row>
-    <row r="43" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B43">
         <v>1.5751299999999999</v>
       </c>
@@ -15128,7 +15152,7 @@
         <v>0.273648</v>
       </c>
     </row>
-    <row r="44" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B44">
         <v>1.5765499999999999</v>
       </c>
@@ -15178,7 +15202,7 @@
         <v>0.27737699999999998</v>
       </c>
     </row>
-    <row r="45" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B45">
         <v>1.57778</v>
       </c>
@@ -15228,7 +15252,7 @@
         <v>0.27992400000000001</v>
       </c>
     </row>
-    <row r="46" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B46">
         <v>1.58544</v>
       </c>
@@ -15278,7 +15302,7 @@
         <v>0.27771000000000001</v>
       </c>
     </row>
-    <row r="47" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B47">
         <v>1.5772200000000001</v>
       </c>
@@ -15328,7 +15352,7 @@
         <v>0.27575699999999997</v>
       </c>
     </row>
-    <row r="48" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B48">
         <v>1.5770999999999999</v>
       </c>
@@ -15378,7 +15402,7 @@
         <v>0.27700200000000003</v>
       </c>
     </row>
-    <row r="49" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B49">
         <v>1.5790900000000001</v>
       </c>
@@ -15428,7 +15452,7 @@
         <v>0.29126999999999997</v>
       </c>
     </row>
-    <row r="50" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B50">
         <v>1.5777000000000001</v>
       </c>
@@ -15478,7 +15502,7 @@
         <v>0.27337400000000001</v>
       </c>
     </row>
-    <row r="51" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B51">
         <v>1.57887</v>
       </c>
@@ -15528,7 +15552,7 @@
         <v>0.276509</v>
       </c>
     </row>
-    <row r="52" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B52">
         <v>1.5728800000000001</v>
       </c>
@@ -15578,7 +15602,7 @@
         <v>0.28887200000000002</v>
       </c>
     </row>
-    <row r="53" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B53">
         <v>1.57792</v>
       </c>
@@ -15628,7 +15652,7 @@
         <v>0.28913899999999998</v>
       </c>
     </row>
-    <row r="54" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B54">
         <v>1.5817600000000001</v>
       </c>
@@ -15678,7 +15702,7 @@
         <v>0.28675200000000001</v>
       </c>
     </row>
-    <row r="55" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B55">
         <v>1.5733200000000001</v>
       </c>
@@ -15728,7 +15752,7 @@
         <v>0.290462</v>
       </c>
     </row>
-    <row r="56" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B56">
         <v>1.5828</v>
       </c>
@@ -15778,7 +15802,7 @@
         <v>0.289186</v>
       </c>
     </row>
-    <row r="57" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B57">
         <v>1.57555</v>
       </c>
@@ -15828,7 +15852,7 @@
         <v>0.28788599999999998</v>
       </c>
     </row>
-    <row r="58" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B58">
         <v>1.57552</v>
       </c>
@@ -15878,7 +15902,7 @@
         <v>0.289904</v>
       </c>
     </row>
-    <row r="59" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B59">
         <v>1.5752600000000001</v>
       </c>
@@ -15928,7 +15952,7 @@
         <v>0.29516300000000001</v>
       </c>
     </row>
-    <row r="60" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B60">
         <v>1.5846899999999999</v>
       </c>
@@ -15978,7 +16002,7 @@
         <v>0.28760599999999997</v>
       </c>
     </row>
-    <row r="61" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B61">
         <v>1.57463</v>
       </c>
@@ -16028,7 +16052,7 @@
         <v>0.27944600000000003</v>
       </c>
     </row>
-    <row r="62" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B62">
         <v>1.5757399999999999</v>
       </c>
@@ -16078,7 +16102,7 @@
         <v>0.279636</v>
       </c>
     </row>
-    <row r="63" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B63">
         <v>1.5782700000000001</v>
       </c>
@@ -16128,7 +16152,7 @@
         <v>0.27872200000000003</v>
       </c>
     </row>
-    <row r="64" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B64">
         <v>1.5800700000000001</v>
       </c>
@@ -16178,7 +16202,7 @@
         <v>0.275001</v>
       </c>
     </row>
-    <row r="65" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B65">
         <v>1.57979</v>
       </c>
@@ -16228,7 +16252,7 @@
         <v>0.27692099999999997</v>
       </c>
     </row>
-    <row r="66" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B66">
         <v>1.58911</v>
       </c>
@@ -16278,7 +16302,7 @@
         <v>0.28206900000000001</v>
       </c>
     </row>
-    <row r="67" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B67">
         <v>1.5969599999999999</v>
       </c>
@@ -16328,7 +16352,7 @@
         <v>0.27749000000000001</v>
       </c>
     </row>
-    <row r="68" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B68">
         <v>1.58789</v>
       </c>
@@ -16378,7 +16402,7 @@
         <v>0.276092</v>
       </c>
     </row>
-    <row r="69" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B69">
         <v>1.5871999999999999</v>
       </c>
@@ -16428,7 +16452,7 @@
         <v>0.27849499999999999</v>
       </c>
     </row>
-    <row r="70" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B70">
         <v>1.5816600000000001</v>
       </c>
@@ -16478,7 +16502,7 @@
         <v>0.28676800000000002</v>
       </c>
     </row>
-    <row r="71" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B71">
         <v>1.5918300000000001</v>
       </c>
@@ -16528,7 +16552,7 @@
         <v>0.27580300000000002</v>
       </c>
     </row>
-    <row r="72" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B72">
         <v>1.5887899999999999</v>
       </c>
@@ -16578,7 +16602,7 @@
         <v>0.27001799999999998</v>
       </c>
     </row>
-    <row r="73" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B73">
         <v>1.5891</v>
       </c>
@@ -16628,7 +16652,7 @@
         <v>0.28292800000000001</v>
       </c>
     </row>
-    <row r="74" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B74">
         <v>1.5842700000000001</v>
       </c>
@@ -16678,7 +16702,7 @@
         <v>0.27837099999999998</v>
       </c>
     </row>
-    <row r="75" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B75">
         <v>1.58586</v>
       </c>
@@ -16728,7 +16752,7 @@
         <v>0.27344600000000002</v>
       </c>
     </row>
-    <row r="76" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B76">
         <v>1.59056</v>
       </c>
@@ -16778,7 +16802,7 @@
         <v>0.27366499999999999</v>
       </c>
     </row>
-    <row r="77" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B77">
         <v>1.5898000000000001</v>
       </c>
@@ -16828,7 +16852,7 @@
         <v>0.28349600000000003</v>
       </c>
     </row>
-    <row r="78" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B78">
         <v>1.58325</v>
       </c>
@@ -16878,7 +16902,7 @@
         <v>0.275704</v>
       </c>
     </row>
-    <row r="79" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B79">
         <v>1.5904</v>
       </c>
@@ -16928,7 +16952,7 @@
         <v>0.27862599999999998</v>
       </c>
     </row>
-    <row r="80" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B80">
         <v>1.5782</v>
       </c>
@@ -16978,7 +17002,7 @@
         <v>0.28200700000000001</v>
       </c>
     </row>
-    <row r="81" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B81">
         <v>1.58507</v>
       </c>
@@ -17028,7 +17052,7 @@
         <v>0.27823399999999998</v>
       </c>
     </row>
-    <row r="82" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B82">
         <v>1.58541</v>
       </c>
@@ -17078,7 +17102,7 @@
         <v>0.279277</v>
       </c>
     </row>
-    <row r="83" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B83">
         <v>1.5924499999999999</v>
       </c>
@@ -17128,7 +17152,7 @@
         <v>0.27470699999999998</v>
       </c>
     </row>
-    <row r="84" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B84">
         <v>1.58212</v>
       </c>
@@ -17178,7 +17202,7 @@
         <v>0.28825200000000001</v>
       </c>
     </row>
-    <row r="85" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B85">
         <v>1.58386</v>
       </c>
@@ -17228,7 +17252,7 @@
         <v>0.276198</v>
       </c>
     </row>
-    <row r="86" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B86">
         <v>1.58162</v>
       </c>
@@ -17278,7 +17302,7 @@
         <v>0.276003</v>
       </c>
     </row>
-    <row r="87" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B87">
         <v>1.58491</v>
       </c>
@@ -17328,7 +17352,7 @@
         <v>0.27904400000000001</v>
       </c>
     </row>
-    <row r="88" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B88">
         <v>1.5873299999999999</v>
       </c>
@@ -17378,7 +17402,7 @@
         <v>0.279972</v>
       </c>
     </row>
-    <row r="89" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B89">
         <v>1.58188</v>
       </c>
@@ -17428,7 +17452,7 @@
         <v>0.275449</v>
       </c>
     </row>
-    <row r="90" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B90">
         <v>1.58487</v>
       </c>
@@ -17478,7 +17502,7 @@
         <v>0.27605400000000002</v>
       </c>
     </row>
-    <row r="91" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B91">
         <v>1.5891299999999999</v>
       </c>
@@ -17528,7 +17552,7 @@
         <v>0.28442099999999998</v>
       </c>
     </row>
-    <row r="92" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B92">
         <v>1.58575</v>
       </c>
@@ -17578,7 +17602,7 @@
         <v>0.27543000000000001</v>
       </c>
     </row>
-    <row r="93" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B93">
         <v>1.58568</v>
       </c>
@@ -17628,7 +17652,7 @@
         <v>0.27789900000000001</v>
       </c>
     </row>
-    <row r="94" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B94">
         <v>1.5860399999999999</v>
       </c>
@@ -17678,7 +17702,7 @@
         <v>0.27564100000000002</v>
       </c>
     </row>
-    <row r="95" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B95">
         <v>1.5844400000000001</v>
       </c>
@@ -17728,7 +17752,7 @@
         <v>0.28144400000000003</v>
       </c>
     </row>
-    <row r="96" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B96">
         <v>1.5809</v>
       </c>
@@ -17778,7 +17802,7 @@
         <v>0.27515499999999998</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B97">
         <v>1.5824800000000001</v>
       </c>
@@ -17828,7 +17852,7 @@
         <v>0.27382699999999999</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B98">
         <v>1.58327</v>
       </c>
@@ -17878,7 +17902,7 @@
         <v>0.27954699999999999</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B99">
         <v>1.58602</v>
       </c>
@@ -17928,7 +17952,7 @@
         <v>0.27729500000000001</v>
       </c>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B100">
         <v>1.59535</v>
       </c>
@@ -17978,7 +18002,7 @@
         <v>0.27522099999999999</v>
       </c>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B101">
         <v>1.58606</v>
       </c>
@@ -18028,7 +18052,7 @@
         <v>0.27845999999999999</v>
       </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B102">
         <v>1.5904100000000001</v>
       </c>
@@ -18078,7 +18102,7 @@
         <v>0.28333799999999998</v>
       </c>
     </row>
-    <row r="103" spans="1:17" ht="21" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:17" ht="21" x14ac:dyDescent="0.65">
       <c r="A103" s="1" t="s">
         <v>9</v>
       </c>
@@ -18147,7 +18171,7 @@
         <v>0.27915175999999997</v>
       </c>
     </row>
-    <row r="104" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:17" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" s="1" t="s">
         <v>10</v>
       </c>
@@ -18228,18 +18252,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFDFEBCA-3C84-4DCF-9E8E-510BA5906146}">
   <dimension ref="A1:Q104"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K119" sqref="K119"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="17" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="17" width="19.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>0</v>
@@ -18290,7 +18314,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
         <v>20</v>
       </c>
@@ -18343,7 +18367,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B3">
         <v>3.0206300000000001</v>
       </c>
@@ -18393,7 +18417,7 @@
         <v>0.488653</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B4">
         <v>3.0207000000000002</v>
       </c>
@@ -18443,7 +18467,7 @@
         <v>0.48118899999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B5">
         <v>3.0209199999999998</v>
       </c>
@@ -18493,7 +18517,7 @@
         <v>0.48716100000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B6">
         <v>3.0153300000000001</v>
       </c>
@@ -18543,7 +18567,7 @@
         <v>0.48556300000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B7">
         <v>3.0299200000000002</v>
       </c>
@@ -18593,7 +18617,7 @@
         <v>0.489817</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B8">
         <v>3.0230600000000001</v>
       </c>
@@ -18643,7 +18667,7 @@
         <v>0.48140500000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B9">
         <v>3.0190800000000002</v>
       </c>
@@ -18693,7 +18717,7 @@
         <v>0.48976599999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B10">
         <v>3.0276399999999999</v>
       </c>
@@ -18743,7 +18767,7 @@
         <v>0.47459499999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B11">
         <v>3.0172099999999999</v>
       </c>
@@ -18793,7 +18817,7 @@
         <v>0.47567900000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B12">
         <v>3.0243600000000002</v>
       </c>
@@ -18843,7 +18867,7 @@
         <v>0.46850399999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B13">
         <v>3.0330400000000002</v>
       </c>
@@ -18893,7 +18917,7 @@
         <v>0.47574300000000003</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B14">
         <v>3.0194000000000001</v>
       </c>
@@ -18943,7 +18967,7 @@
         <v>0.47192699999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B15">
         <v>3.0319400000000001</v>
       </c>
@@ -18993,7 +19017,7 @@
         <v>0.47541299999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B16">
         <v>3.0142199999999999</v>
       </c>
@@ -19043,7 +19067,7 @@
         <v>0.469781</v>
       </c>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B17">
         <v>3.0248300000000001</v>
       </c>
@@ -19093,7 +19117,7 @@
         <v>0.487738</v>
       </c>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B18">
         <v>3.01295</v>
       </c>
@@ -19143,7 +19167,7 @@
         <v>0.48477900000000002</v>
       </c>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B19">
         <v>3.0038499999999999</v>
       </c>
@@ -19193,7 +19217,7 @@
         <v>0.48846899999999999</v>
       </c>
     </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B20">
         <v>3.03559</v>
       </c>
@@ -19243,7 +19267,7 @@
         <v>0.482765</v>
       </c>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B21">
         <v>3.0179399999999998</v>
       </c>
@@ -19293,7 +19317,7 @@
         <v>0.48045100000000002</v>
       </c>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B22">
         <v>3.0235599999999998</v>
       </c>
@@ -19343,7 +19367,7 @@
         <v>0.47210600000000003</v>
       </c>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B23">
         <v>3.0182500000000001</v>
       </c>
@@ -19393,7 +19417,7 @@
         <v>0.46843400000000002</v>
       </c>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B24">
         <v>3.0248599999999999</v>
       </c>
@@ -19443,7 +19467,7 @@
         <v>0.45955000000000001</v>
       </c>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B25">
         <v>3.0255000000000001</v>
       </c>
@@ -19493,7 +19517,7 @@
         <v>0.45724799999999999</v>
       </c>
     </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B26">
         <v>3.0200200000000001</v>
       </c>
@@ -19543,7 +19567,7 @@
         <v>0.47099800000000003</v>
       </c>
     </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B27">
         <v>3.0356299999999998</v>
       </c>
@@ -19593,7 +19617,7 @@
         <v>0.461005</v>
       </c>
     </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B28">
         <v>3.0298600000000002</v>
       </c>
@@ -19643,7 +19667,7 @@
         <v>0.46613199999999999</v>
       </c>
     </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B29">
         <v>3.0244499999999999</v>
       </c>
@@ -19693,7 +19717,7 @@
         <v>0.455729</v>
       </c>
     </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B30">
         <v>3.0179200000000002</v>
       </c>
@@ -19743,7 +19767,7 @@
         <v>0.47168199999999999</v>
       </c>
     </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B31">
         <v>3.0345900000000001</v>
       </c>
@@ -19793,7 +19817,7 @@
         <v>0.47332299999999999</v>
       </c>
     </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B32">
         <v>3.0251800000000002</v>
       </c>
@@ -19843,7 +19867,7 @@
         <v>0.47706100000000001</v>
       </c>
     </row>
-    <row r="33" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B33">
         <v>3.0162399999999998</v>
       </c>
@@ -19893,7 +19917,7 @@
         <v>0.46765600000000002</v>
       </c>
     </row>
-    <row r="34" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B34">
         <v>3.0177800000000001</v>
       </c>
@@ -19943,7 +19967,7 @@
         <v>0.47779100000000002</v>
       </c>
     </row>
-    <row r="35" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B35">
         <v>3.0244</v>
       </c>
@@ -19993,7 +20017,7 @@
         <v>0.47138600000000003</v>
       </c>
     </row>
-    <row r="36" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B36">
         <v>3.02156</v>
       </c>
@@ -20043,7 +20067,7 @@
         <v>0.47567399999999999</v>
       </c>
     </row>
-    <row r="37" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B37">
         <v>3.02128</v>
       </c>
@@ -20093,7 +20117,7 @@
         <v>0.46816400000000002</v>
       </c>
     </row>
-    <row r="38" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B38">
         <v>3.0230000000000001</v>
       </c>
@@ -20143,7 +20167,7 @@
         <v>0.48149999999999998</v>
       </c>
     </row>
-    <row r="39" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B39">
         <v>3.02122</v>
       </c>
@@ -20193,7 +20217,7 @@
         <v>0.48694999999999999</v>
       </c>
     </row>
-    <row r="40" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B40">
         <v>3.03234</v>
       </c>
@@ -20243,7 +20267,7 @@
         <v>0.48763600000000001</v>
       </c>
     </row>
-    <row r="41" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B41">
         <v>3.0242599999999999</v>
       </c>
@@ -20293,7 +20317,7 @@
         <v>0.482433</v>
       </c>
     </row>
-    <row r="42" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B42">
         <v>3.0092699999999999</v>
       </c>
@@ -20343,7 +20367,7 @@
         <v>0.47625600000000001</v>
       </c>
     </row>
-    <row r="43" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B43">
         <v>3.00651</v>
       </c>
@@ -20393,7 +20417,7 @@
         <v>0.481209</v>
       </c>
     </row>
-    <row r="44" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B44">
         <v>3.0081899999999999</v>
       </c>
@@ -20443,7 +20467,7 @@
         <v>0.46793499999999999</v>
       </c>
     </row>
-    <row r="45" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B45">
         <v>3.0095700000000001</v>
       </c>
@@ -20493,7 +20517,7 @@
         <v>0.46808</v>
       </c>
     </row>
-    <row r="46" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B46">
         <v>3.0184500000000001</v>
       </c>
@@ -20543,7 +20567,7 @@
         <v>0.47164</v>
       </c>
     </row>
-    <row r="47" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B47">
         <v>3.0042599999999999</v>
       </c>
@@ -20593,7 +20617,7 @@
         <v>0.47636400000000001</v>
       </c>
     </row>
-    <row r="48" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B48">
         <v>3.0051000000000001</v>
       </c>
@@ -20643,7 +20667,7 @@
         <v>0.47312500000000002</v>
       </c>
     </row>
-    <row r="49" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B49">
         <v>3.0054400000000001</v>
       </c>
@@ -20693,7 +20717,7 @@
         <v>0.47524</v>
       </c>
     </row>
-    <row r="50" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B50">
         <v>3.0200900000000002</v>
       </c>
@@ -20743,7 +20767,7 @@
         <v>0.46914</v>
       </c>
     </row>
-    <row r="51" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B51">
         <v>3.0202499999999999</v>
       </c>
@@ -20793,7 +20817,7 @@
         <v>0.47433999999999998</v>
       </c>
     </row>
-    <row r="52" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B52">
         <v>3.0134300000000001</v>
       </c>
@@ -20843,7 +20867,7 @@
         <v>0.46060699999999999</v>
       </c>
     </row>
-    <row r="53" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B53">
         <v>3.0174099999999999</v>
       </c>
@@ -20893,7 +20917,7 @@
         <v>0.46064300000000002</v>
       </c>
     </row>
-    <row r="54" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B54">
         <v>3.0218600000000002</v>
       </c>
@@ -20943,7 +20967,7 @@
         <v>0.45550299999999999</v>
       </c>
     </row>
-    <row r="55" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B55">
         <v>3.02582</v>
       </c>
@@ -20993,7 +21017,7 @@
         <v>0.46233600000000002</v>
       </c>
     </row>
-    <row r="56" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B56">
         <v>3.0170300000000001</v>
       </c>
@@ -21043,7 +21067,7 @@
         <v>0.49665500000000001</v>
       </c>
     </row>
-    <row r="57" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B57">
         <v>3.0280300000000002</v>
       </c>
@@ -21093,7 +21117,7 @@
         <v>0.52323699999999995</v>
       </c>
     </row>
-    <row r="58" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B58">
         <v>3.0227900000000001</v>
       </c>
@@ -21143,7 +21167,7 @@
         <v>0.51902300000000001</v>
       </c>
     </row>
-    <row r="59" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B59">
         <v>3.0212300000000001</v>
       </c>
@@ -21193,7 +21217,7 @@
         <v>0.52903</v>
       </c>
     </row>
-    <row r="60" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B60">
         <v>3.0242599999999999</v>
       </c>
@@ -21243,7 +21267,7 @@
         <v>0.46502500000000002</v>
       </c>
     </row>
-    <row r="61" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B61">
         <v>3.0234999999999999</v>
       </c>
@@ -21293,7 +21317,7 @@
         <v>0.464366</v>
       </c>
     </row>
-    <row r="62" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B62">
         <v>3.0228700000000002</v>
       </c>
@@ -21343,7 +21367,7 @@
         <v>0.46694999999999998</v>
       </c>
     </row>
-    <row r="63" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B63">
         <v>3.01986</v>
       </c>
@@ -21393,7 +21417,7 @@
         <v>0.47197099999999997</v>
       </c>
     </row>
-    <row r="64" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B64">
         <v>3.0219100000000001</v>
       </c>
@@ -21443,7 +21467,7 @@
         <v>0.46204899999999999</v>
       </c>
     </row>
-    <row r="65" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B65">
         <v>3.0213800000000002</v>
       </c>
@@ -21493,7 +21517,7 @@
         <v>0.456063</v>
       </c>
     </row>
-    <row r="66" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B66">
         <v>3.0173100000000002</v>
       </c>
@@ -21543,7 +21567,7 @@
         <v>0.46077200000000001</v>
       </c>
     </row>
-    <row r="67" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B67">
         <v>3.0231699999999999</v>
       </c>
@@ -21593,7 +21617,7 @@
         <v>0.46166099999999999</v>
       </c>
     </row>
-    <row r="68" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B68">
         <v>3.0209700000000002</v>
       </c>
@@ -21643,7 +21667,7 @@
         <v>0.47529500000000002</v>
       </c>
     </row>
-    <row r="69" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B69">
         <v>3.01831</v>
       </c>
@@ -21693,7 +21717,7 @@
         <v>0.45957199999999998</v>
       </c>
     </row>
-    <row r="70" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B70">
         <v>3.0200499999999999</v>
       </c>
@@ -21743,7 +21767,7 @@
         <v>0.46409899999999998</v>
       </c>
     </row>
-    <row r="71" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B71">
         <v>3.0202300000000002</v>
       </c>
@@ -21793,7 +21817,7 @@
         <v>0.45566800000000002</v>
       </c>
     </row>
-    <row r="72" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B72">
         <v>3.0127700000000002</v>
       </c>
@@ -21843,7 +21867,7 @@
         <v>0.46227699999999999</v>
       </c>
     </row>
-    <row r="73" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B73">
         <v>3.0177299999999998</v>
       </c>
@@ -21893,7 +21917,7 @@
         <v>0.45690700000000001</v>
       </c>
     </row>
-    <row r="74" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B74">
         <v>3.0212500000000002</v>
       </c>
@@ -21943,7 +21967,7 @@
         <v>0.46799499999999999</v>
       </c>
     </row>
-    <row r="75" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B75">
         <v>3.0159600000000002</v>
       </c>
@@ -21993,7 +22017,7 @@
         <v>0.45421699999999998</v>
       </c>
     </row>
-    <row r="76" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B76">
         <v>3.0198900000000002</v>
       </c>
@@ -22043,7 +22067,7 @@
         <v>0.44946700000000001</v>
       </c>
     </row>
-    <row r="77" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B77">
         <v>3.01966</v>
       </c>
@@ -22093,7 +22117,7 @@
         <v>0.44578800000000002</v>
       </c>
     </row>
-    <row r="78" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B78">
         <v>3.0199500000000001</v>
       </c>
@@ -22143,7 +22167,7 @@
         <v>0.45350200000000002</v>
       </c>
     </row>
-    <row r="79" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B79">
         <v>3.0026899999999999</v>
       </c>
@@ -22193,7 +22217,7 @@
         <v>0.46421200000000001</v>
       </c>
     </row>
-    <row r="80" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B80">
         <v>3.00414</v>
       </c>
@@ -22243,7 +22267,7 @@
         <v>0.45874100000000001</v>
       </c>
     </row>
-    <row r="81" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B81">
         <v>3.0052500000000002</v>
       </c>
@@ -22293,7 +22317,7 @@
         <v>0.46712500000000001</v>
       </c>
     </row>
-    <row r="82" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B82">
         <v>3.00604</v>
       </c>
@@ -22343,7 +22367,7 @@
         <v>0.460507</v>
       </c>
     </row>
-    <row r="83" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B83">
         <v>3.0094500000000002</v>
       </c>
@@ -22393,7 +22417,7 @@
         <v>0.464895</v>
       </c>
     </row>
-    <row r="84" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B84">
         <v>3.0212400000000001</v>
       </c>
@@ -22443,7 +22467,7 @@
         <v>0.457536</v>
       </c>
     </row>
-    <row r="85" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B85">
         <v>3.0069300000000001</v>
       </c>
@@ -22493,7 +22517,7 @@
         <v>0.46299299999999999</v>
       </c>
     </row>
-    <row r="86" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B86">
         <v>3.00895</v>
       </c>
@@ -22543,7 +22567,7 @@
         <v>0.45885900000000002</v>
       </c>
     </row>
-    <row r="87" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B87">
         <v>3.0154299999999998</v>
       </c>
@@ -22593,7 +22617,7 @@
         <v>0.46106799999999998</v>
       </c>
     </row>
-    <row r="88" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B88">
         <v>3.0196200000000002</v>
       </c>
@@ -22643,7 +22667,7 @@
         <v>0.46665000000000001</v>
       </c>
     </row>
-    <row r="89" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B89">
         <v>3.00217</v>
       </c>
@@ -22693,7 +22717,7 @@
         <v>0.46064100000000002</v>
       </c>
     </row>
-    <row r="90" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B90">
         <v>3.0133299999999998</v>
       </c>
@@ -22743,7 +22767,7 @@
         <v>0.458422</v>
       </c>
     </row>
-    <row r="91" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B91">
         <v>3.0162300000000002</v>
       </c>
@@ -22793,7 +22817,7 @@
         <v>0.460397</v>
       </c>
     </row>
-    <row r="92" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B92">
         <v>3.0220600000000002</v>
       </c>
@@ -22843,7 +22867,7 @@
         <v>0.45965699999999998</v>
       </c>
     </row>
-    <row r="93" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B93">
         <v>3.0334699999999999</v>
       </c>
@@ -22893,7 +22917,7 @@
         <v>0.454542</v>
       </c>
     </row>
-    <row r="94" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B94">
         <v>3.0183499999999999</v>
       </c>
@@ -22943,7 +22967,7 @@
         <v>0.46191399999999999</v>
       </c>
     </row>
-    <row r="95" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B95">
         <v>3.0162900000000001</v>
       </c>
@@ -22993,7 +23017,7 @@
         <v>0.45664500000000002</v>
       </c>
     </row>
-    <row r="96" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B96">
         <v>3.03125</v>
       </c>
@@ -23043,7 +23067,7 @@
         <v>0.46194099999999999</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B97">
         <v>3.0283799999999998</v>
       </c>
@@ -23093,7 +23117,7 @@
         <v>0.457256</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B98">
         <v>3.0253700000000001</v>
       </c>
@@ -23143,7 +23167,7 @@
         <v>0.46201999999999999</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B99">
         <v>3.01044</v>
       </c>
@@ -23193,7 +23217,7 @@
         <v>0.45596999999999999</v>
       </c>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B100">
         <v>3.0188000000000001</v>
       </c>
@@ -23243,7 +23267,7 @@
         <v>0.45318999999999998</v>
       </c>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B101">
         <v>3.0146600000000001</v>
       </c>
@@ -23293,7 +23317,7 @@
         <v>0.45495799999999997</v>
       </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B102">
         <v>3.01911</v>
       </c>
@@ -23343,7 +23367,7 @@
         <v>0.46056000000000002</v>
       </c>
     </row>
-    <row r="103" spans="1:17" ht="21" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:17" ht="21" x14ac:dyDescent="0.65">
       <c r="A103" s="1" t="s">
         <v>9</v>
       </c>
@@ -23412,7 +23436,7 @@
         <v>0.47006562000000024</v>
       </c>
     </row>
-    <row r="104" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:17" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" s="1" t="s">
         <v>10</v>
       </c>

</xml_diff>